<commit_message>
Understanding how to reverse LinkedList
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -139,13 +139,13 @@
     <t>Not Sure</t>
   </si>
   <si>
-    <t>Best Time to Buy and Sell Stock</t>
+    <t>*Best Time to Buy and Sell Stock</t>
   </si>
   <si>
     <t>Adobe, Alation, Amazon, Apple, Atlassian, Bloomberg, ByteDance, Capital One, Cisco, Docusign, Expedia, Goldman Sachs, JP Morgan, Netflix, Orcale, Paypal, ServiceNow, Uber, Visa, Walmart, Zoho, Zoom, eBay, tcs</t>
   </si>
   <si>
-    <t xml:space="preserve">Snapshot Array </t>
+    <t xml:space="preserve">*Snapshot Array </t>
   </si>
   <si>
     <t>Medium</t>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">Binary Search </t>
   </si>
   <si>
-    <t>Reverse Linked List</t>
+    <t>*Reverse Linked List</t>
   </si>
   <si>
     <t>Intuit, Yandex</t>
@@ -1126,7 +1126,9 @@
       <c r="D18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>

</xml_diff>

<commit_message>
Added merge two sorted list (incomplete)
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="59">
   <si>
     <t>Src</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Create Binary Tree</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t>Accenture, Adobe, Orcale, Shoppe</t>
   </si>
 </sst>
 </file>
@@ -834,8 +840,8 @@
       <c r="D6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="8">
-        <v>2</v>
+      <c r="E6" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="F6" s="8">
         <v>1</v>
@@ -1236,10 +1242,18 @@
       <c r="N20" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>

</xml_diff>

<commit_message>
Updated Random Question Database
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="60">
   <si>
     <t>Src</t>
   </si>
@@ -145,13 +145,13 @@
     <t>Not Sure</t>
   </si>
   <si>
-    <t>*Best Time to Buy and Sell Stock</t>
+    <t>Best Time to Buy and Sell Stock</t>
   </si>
   <si>
     <t>Adobe, Alation, Amazon, Apple, Atlassian, Bloomberg, ByteDance, Capital One, Cisco, Docusign, Expedia, Goldman Sachs, JP Morgan, Netflix, Orcale, Paypal, ServiceNow, Uber, Visa, Walmart, Zoho, Zoom, eBay, tcs</t>
   </si>
   <si>
-    <t xml:space="preserve">*Snapshot Array </t>
+    <t xml:space="preserve">Snapshot Array </t>
   </si>
   <si>
     <t>Medium</t>
@@ -163,7 +163,7 @@
     <t xml:space="preserve">Binary Search </t>
   </si>
   <si>
-    <t>*Reverse Linked List</t>
+    <t>Reverse Linked List (Iteratively)</t>
   </si>
   <si>
     <t>Intuit, Yandex</t>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>Accenture, Adobe, Orcale, Shoppe</t>
+  </si>
+  <si>
+    <t>Reverse Linked List (Recursively)</t>
   </si>
 </sst>
 </file>
@@ -1174,8 +1177,8 @@
       <c r="D18" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="8">
-        <v>3</v>
+      <c r="E18" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1227,7 +1230,9 @@
       <c r="C20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="E20" s="8">
         <v>1</v>
       </c>
@@ -1266,10 +1271,18 @@
       <c r="N21" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
+      <c r="A22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>

</xml_diff>

<commit_message>
reattempt merge two linkedlist
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="60">
   <si>
     <t>Src</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>Palindrome Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Merge Two Sorted List </t>
   </si>
   <si>
     <t xml:space="preserve">Happy Number </t>
@@ -635,7 +632,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N1001"/>
+  <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -657,7 +654,7 @@
     <col min="14" max="14" style="10" width="16.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -701,7 +698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -805,7 +802,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -833,7 +830,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -861,7 +858,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -889,7 +886,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -919,7 +916,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -947,24 +944,24 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E10" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="9"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -973,21 +970,21 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
-      <c r="E11" s="8">
-        <v>3</v>
+      <c r="E11" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -997,23 +994,25 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="N11" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1024,24 +1023,24 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="6" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1052,24 +1051,24 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1080,26 +1079,28 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>28</v>
+      <c r="E15" s="8">
+        <v>2</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="8">
+        <v>1</v>
+      </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="1"/>
@@ -1107,29 +1108,25 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="N15" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
-      <c r="E16" s="8">
-        <v>2</v>
+      <c r="E16" s="8" t="s">
+        <v>38</v>
       </c>
-      <c r="F16" s="8">
-        <v>1</v>
-      </c>
+      <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
@@ -1137,9 +1134,11 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="N16" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1150,69 +1149,67 @@
         <v>17</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="6" t="s">
-        <v>43</v>
+      <c r="K17" s="6" t="s">
+        <v>51</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="L17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N17" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="8">
+        <v>2</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1223,18 +1220,18 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="E20" s="8">
         <v>2</v>
@@ -1249,18 +1246,18 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1273,19 +1270,11 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>51</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1297,7 +1286,7 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="6"/>
@@ -1313,7 +1302,7 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="6"/>
@@ -1409,7 +1398,7 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="6"/>
@@ -1425,7 +1414,7 @@
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="6"/>
@@ -1441,7 +1430,7 @@
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="6"/>
@@ -1457,7 +1446,7 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="6"/>
@@ -1473,7 +1462,7 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="6"/>
@@ -1489,7 +1478,7 @@
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="6"/>
@@ -1505,7 +1494,7 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="6"/>
@@ -1553,7 +1542,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="6"/>
@@ -16945,22 +16934,6 @@
       <c r="M1000" s="1"/>
       <c r="N1000" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="1001" customHeight="1" ht="17.25">
-      <c r="A1001" s="1"/>
-      <c r="B1001" s="1"/>
-      <c r="C1001" s="6"/>
-      <c r="D1001" s="6"/>
-      <c r="E1001" s="3"/>
-      <c r="F1001" s="3"/>
-      <c r="G1001" s="3"/>
-      <c r="H1001" s="3"/>
-      <c r="I1001" s="1"/>
-      <c r="J1001" s="1"/>
-      <c r="K1001" s="1"/>
-      <c r="L1001" s="1"/>
-      <c r="M1001" s="1"/>
-      <c r="N1001" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added hasCycle to LinkedListV1.py
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
   <si>
     <t>Src</t>
   </si>
@@ -169,6 +169,9 @@
     <t>Intuit, Yandex</t>
   </si>
   <si>
+    <t>4*</t>
+  </si>
+  <si>
     <t xml:space="preserve">O(n) - Will grow linearly and in direct proportion to the size of the input data </t>
   </si>
   <si>
@@ -194,6 +197,15 @@
   </si>
   <si>
     <t>Reverse Linked List (Recursively)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has Cycle </t>
+  </si>
+  <si>
+    <t>O(n)</t>
+  </si>
+  <si>
+    <t>O(1)</t>
   </si>
 </sst>
 </file>
@@ -654,7 +666,7 @@
     <col min="14" max="14" style="10" width="16.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +710,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +814,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -830,7 +842,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -858,7 +870,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -886,7 +898,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -916,7 +928,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -944,7 +956,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -970,7 +982,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -998,7 +1010,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1026,7 +1038,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1054,7 +1066,7 @@
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1082,7 +1094,7 @@
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1110,7 +1122,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1138,7 +1150,7 @@
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1152,7 +1164,7 @@
         <v>50</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1160,22 +1172,22 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N17" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>17</v>
@@ -1194,12 +1206,12 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>18</v>
@@ -1220,18 +1232,18 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E20" s="8">
         <v>2</v>
@@ -1246,12 +1258,12 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>17</v>
@@ -1270,23 +1282,37 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="6"/>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="D22" s="6"/>
-      <c r="E22" s="3"/>
+      <c r="E22" s="8">
+        <v>1</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="K22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="N22" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="6"/>
@@ -1302,7 +1328,7 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="6"/>
@@ -1318,7 +1344,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="6"/>
@@ -1334,7 +1360,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="6"/>
@@ -1350,7 +1376,7 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="6"/>
@@ -1366,7 +1392,7 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="6"/>
@@ -1382,7 +1408,7 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="6"/>

</xml_diff>

<commit_message>
added: contains duplicate to JS folder
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
   <si>
     <t>Src</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t xml:space="preserve">Has Cycle </t>
+  </si>
+  <si>
+    <t>Spotify(4), Visa(3)</t>
   </si>
   <si>
     <t>O(n)</t>
@@ -1292,7 +1295,9 @@
       <c r="C22" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="E22" s="8">
         <v>1</v>
       </c>
@@ -1302,10 +1307,10 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="6" t="s">

</xml_diff>

<commit_message>
Reattemp has cycle in linkedlist
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -100,9 +100,6 @@
     <t xml:space="preserve">Create LinkedList from scratch </t>
   </si>
   <si>
-    <t>2*</t>
-  </si>
-  <si>
     <t xml:space="preserve">First Bad Version </t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>Palindrome Number</t>
+  </si>
+  <si>
+    <t>2*</t>
   </si>
   <si>
     <t xml:space="preserve">Happy Number </t>
@@ -169,7 +169,7 @@
     <t>Intuit, Yandex</t>
   </si>
   <si>
-    <t>4*</t>
+    <t>5*</t>
   </si>
   <si>
     <t xml:space="preserve">O(n) - Will grow linearly and in direct proportion to the size of the input data </t>
@@ -887,7 +887,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F7" s="8">
         <v>1</v>
@@ -906,13 +906,13 @@
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>21</v>
@@ -936,7 +936,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>17</v>
@@ -945,7 +945,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="8">
@@ -999,7 +999,7 @@
         <v>35</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -1083,7 +1083,7 @@
         <v>44</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1139,7 +1139,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -1249,7 +1249,7 @@
         <v>59</v>
       </c>
       <c r="E20" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>

</xml_diff>

<commit_message>
Added reverse linkedlist recursively
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -1274,7 +1274,9 @@
       <c r="D21" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>

</xml_diff>

<commit_message>
Reattempt: Contains Duplicate and Best Time to Buy
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -999,7 +999,7 @@
         <v>35</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -1083,7 +1083,7 @@
         <v>44</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>

</xml_diff>

<commit_message>
Reattempt LinkedList with relevant methods
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
   <si>
     <t>Src</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Accenture, Adobe, Orcale, Shoppe</t>
+  </si>
+  <si>
+    <t>4*</t>
   </si>
   <si>
     <t>Reverse Linked List (Recursively)</t>
@@ -1248,8 +1251,8 @@
       <c r="D20" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="8">
-        <v>3</v>
+      <c r="E20" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1266,7 +1269,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>17</v>
@@ -1274,7 +1277,7 @@
       <c r="D21" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="8">
         <v>1</v>
       </c>
       <c r="F21" s="3"/>
@@ -1292,16 +1295,16 @@
         <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E22" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1309,10 +1312,10 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="6" t="s">

</xml_diff>

<commit_message>
Attempt at Invert Binary Tree
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="67">
   <si>
     <t>Src</t>
   </si>
@@ -151,6 +151,9 @@
     <t>Adobe, Alation, Amazon, Apple, Atlassian, Bloomberg, ByteDance, Capital One, Cisco, Docusign, Expedia, Goldman Sachs, JP Morgan, Netflix, Orcale, Paypal, ServiceNow, Uber, Visa, Walmart, Zoho, Zoom, eBay, tcs</t>
   </si>
   <si>
+    <t>4*</t>
+  </si>
+  <si>
     <t xml:space="preserve">Snapshot Array </t>
   </si>
   <si>
@@ -169,7 +172,7 @@
     <t>Intuit, Yandex</t>
   </si>
   <si>
-    <t>5*</t>
+    <t>6*</t>
   </si>
   <si>
     <t xml:space="preserve">O(n) - Will grow linearly and in direct proportion to the size of the input data </t>
@@ -194,9 +197,6 @@
   </si>
   <si>
     <t>Accenture, Adobe, Orcale, Shoppe</t>
-  </si>
-  <si>
-    <t>4*</t>
   </si>
   <si>
     <t>Reverse Linked List (Recursively)</t>
@@ -1089,7 +1089,7 @@
         <v>44</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1108,13 +1108,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E15" s="8">
         <v>2</v>
@@ -1136,7 +1136,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>17</v>
@@ -1164,16 +1164,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1181,22 +1181,22 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N17" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>17</v>
@@ -1204,7 +1204,9 @@
       <c r="D18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1220,7 +1222,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>18</v>
@@ -1246,16 +1248,16 @@
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1278,10 +1280,10 @@
         <v>17</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
-      <c r="E21" s="8">
-        <v>1</v>
+      <c r="E21" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -1306,8 +1308,8 @@
       <c r="D22" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E22" s="8">
-        <v>2</v>
+      <c r="E22" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1338,7 +1340,7 @@
       <c r="D23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="8">
         <v>1</v>
       </c>
       <c r="F23" s="3"/>

</xml_diff>

<commit_message>
Added: Maximum Depth of Binary Tree
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="71">
   <si>
     <t>Src</t>
   </si>
@@ -215,6 +215,18 @@
   </si>
   <si>
     <t xml:space="preserve">Factorial Recursive </t>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree (Recursive)</t>
+  </si>
+  <si>
+    <t>Spotify(4)</t>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree (DFS)</t>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree (BFS)</t>
   </si>
 </sst>
 </file>
@@ -660,7 +672,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="10" width="5.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="28.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="40.14785714285715" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="11" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="11" width="31.005" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="12" width="8.290714285714287" customWidth="1" bestFit="1"/>
@@ -1204,8 +1216,8 @@
       <c r="D18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="3">
-        <v>1</v>
+      <c r="E18" s="8">
+        <v>2</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1354,11 +1366,21 @@
       <c r="N23" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="3"/>
+      <c r="A24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="8">
+        <v>1</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1370,11 +1392,21 @@
       <c r="N24" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="3"/>
+      <c r="A25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="8">
+        <v>1</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1386,11 +1418,21 @@
       <c r="N25" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="3"/>
+      <c r="A26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="8">
+        <v>1</v>
+      </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>

</xml_diff>

<commit_message>
Reattemp at creating and inverting Binary Tree
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="74">
   <si>
     <t>Src</t>
   </si>
@@ -166,6 +166,15 @@
     <t xml:space="preserve">Binary Search </t>
   </si>
   <si>
+    <t xml:space="preserve">O(logN) - The element is to search is in the first index or last index
+In this case, the total number of comparisons required is logN comparisons.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O(1) - This is because we need two variable to keep track of the range of elements that are to be checked. No other data is needed.
+</t>
+  </si>
+  <si>
     <t>Reverse Linked List (Iteratively)</t>
   </si>
   <si>
@@ -227,6 +236,9 @@
   </si>
   <si>
     <t>Maximum Depth of Binary Tree (BFS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary Search Recursion </t>
   </si>
 </sst>
 </file>
@@ -1157,15 +1169,19 @@
         <v>18</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="K16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="M16" s="1"/>
       <c r="N16" s="6" t="s">
         <v>42</v>
@@ -1176,16 +1192,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1193,22 +1209,22 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N17" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>17</v>
@@ -1217,7 +1233,7 @@
         <v>18</v>
       </c>
       <c r="E18" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1234,7 +1250,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>18</v>
@@ -1243,7 +1259,7 @@
         <v>18</v>
       </c>
       <c r="E19" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1260,13 +1276,13 @@
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>45</v>
@@ -1286,13 +1302,13 @@
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>31</v>
@@ -1312,13 +1328,13 @@
         <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>21</v>
@@ -1329,10 +1345,10 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="6" t="s">
@@ -1344,7 +1360,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>18</v>
@@ -1370,13 +1386,13 @@
         <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E24" s="8">
         <v>1</v>
@@ -1396,13 +1412,13 @@
         <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E25" s="8">
         <v>1</v>
@@ -1422,13 +1438,13 @@
         <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E26" s="8">
         <v>1</v>
@@ -1444,10 +1460,18 @@
       <c r="N26" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>

</xml_diff>

<commit_message>
reattempt: creating binary tree
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -1155,7 +1155,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>18</v>
       </c>
       <c r="E18" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1259,7 +1259,7 @@
         <v>18</v>
       </c>
       <c r="E19" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1337,7 +1337,7 @@
         <v>65</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>

</xml_diff>

<commit_message>
reattempt creating LinkedList from scratch
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -100,13 +100,16 @@
     <t xml:space="preserve">Create LinkedList from scratch </t>
   </si>
   <si>
-    <t>4*</t>
+    <t>5*</t>
   </si>
   <si>
     <t xml:space="preserve">First Bad Version </t>
   </si>
   <si>
     <t>Google</t>
+  </si>
+  <si>
+    <t>4*</t>
   </si>
   <si>
     <t>Palindrome Number</t>
@@ -181,7 +184,7 @@
     <t>Intuit, Yandex</t>
   </si>
   <si>
-    <t>7*</t>
+    <t>8*</t>
   </si>
   <si>
     <t xml:space="preserve">O(n) - Will grow linearly and in direct proportion to the size of the input data </t>
@@ -206,9 +209,6 @@
   </si>
   <si>
     <t>Accenture, Adobe, Orcale, Shoppe</t>
-  </si>
-  <si>
-    <t>5*</t>
   </si>
   <si>
     <t>Reverse Linked List (Recursively)</t>
@@ -948,7 +948,7 @@
         <v>30</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F8" s="8">
         <v>1</v>
@@ -969,7 +969,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>17</v>
@@ -978,7 +978,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="8">
@@ -997,13 +997,13 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="8">
         <v>3</v>
@@ -1023,13 +1023,13 @@
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>21</v>
@@ -1051,16 +1051,16 @@
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1071,7 +1071,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -1079,16 +1079,16 @@
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1099,7 +1099,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
@@ -1107,16 +1107,16 @@
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1127,7 +1127,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
@@ -1135,13 +1135,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E15" s="8">
         <v>2</v>
@@ -1158,12 +1158,12 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>17</v>
@@ -1180,14 +1180,14 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
@@ -1195,16 +1195,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1212,22 +1212,22 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N17" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>17</v>
@@ -1253,7 +1253,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>18</v>
@@ -1279,16 +1279,16 @@
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1311,7 +1311,7 @@
         <v>17</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>21</v>
@@ -1340,7 +1340,7 @@
         <v>66</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1518,7 +1518,7 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="6"/>

</xml_diff>

<commit_message>
added: break a palindrome
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="76">
   <si>
     <t>Src</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t xml:space="preserve">Binary Search Recursion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Break a palindrome </t>
   </si>
 </sst>
 </file>
@@ -1487,17 +1490,29 @@
       <c r="N27" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="3"/>
+      <c r="A28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
+      <c r="K28" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>

</xml_diff>

<commit_message>
reattempt snap shot array and first bad version
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="76">
   <si>
     <t>Src</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Google</t>
   </si>
   <si>
-    <t>4*</t>
-  </si>
-  <si>
     <t>Palindrome Number</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>Adobe, Alation, Amazon, Apple, Atlassian, Bloomberg, ByteDance, Capital One, Cisco, Docusign, Expedia, Goldman Sachs, JP Morgan, Netflix, Orcale, Paypal, ServiceNow, Uber, Visa, Walmart, Zoho, Zoom, eBay, tcs</t>
+  </si>
+  <si>
+    <t>4*</t>
   </si>
   <si>
     <t xml:space="preserve">Snapshot Array </t>
@@ -951,7 +951,7 @@
         <v>30</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F8" s="8">
         <v>1</v>
@@ -972,7 +972,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>17</v>
@@ -981,7 +981,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="8">
@@ -1000,13 +1000,13 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="8">
         <v>3</v>
@@ -1026,13 +1026,13 @@
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>21</v>
@@ -1054,16 +1054,16 @@
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1074,7 +1074,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -1082,16 +1082,16 @@
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1102,7 +1102,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
@@ -1110,16 +1110,16 @@
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1130,7 +1130,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
@@ -1147,7 +1147,7 @@
         <v>49</v>
       </c>
       <c r="E15" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="8">
         <v>1</v>
@@ -1161,7 +1161,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="44.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
@@ -1401,14 +1401,16 @@
         <v>71</v>
       </c>
       <c r="E24" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
+      <c r="K24" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1460,7 +1462,9 @@
       <c r="H26" s="3"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
+      <c r="K26" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -1502,7 +1506,7 @@
       <c r="D28" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="8">
         <v>1</v>
       </c>
       <c r="F28" s="3"/>
@@ -1549,7 +1553,7 @@
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="6"/>
@@ -1565,7 +1569,7 @@
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="6"/>
@@ -1581,7 +1585,7 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="6"/>
@@ -1597,7 +1601,7 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="6"/>

</xml_diff>

<commit_message>
creating linkedlist from sratch
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="78">
   <si>
     <t>Src</t>
   </si>
@@ -100,13 +100,16 @@
     <t xml:space="preserve">Create LinkedList from scratch </t>
   </si>
   <si>
-    <t>5*</t>
+    <t>6*</t>
   </si>
   <si>
     <t xml:space="preserve">First Bad Version </t>
   </si>
   <si>
     <t>Google</t>
+  </si>
+  <si>
+    <t>5*</t>
   </si>
   <si>
     <t>Palindrome Number</t>
@@ -954,7 +957,7 @@
         <v>30</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F8" s="8">
         <v>1</v>
@@ -975,7 +978,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>17</v>
@@ -984,7 +987,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="8">
@@ -1003,13 +1006,13 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="8">
         <v>3</v>
@@ -1029,13 +1032,13 @@
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>21</v>
@@ -1057,16 +1060,16 @@
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1077,7 +1080,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -1085,16 +1088,16 @@
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1105,7 +1108,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
@@ -1113,16 +1116,16 @@
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1133,7 +1136,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
@@ -1141,13 +1144,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E15" s="8">
         <v>3</v>
@@ -1169,7 +1172,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>17</v>
@@ -1186,14 +1189,14 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
@@ -1201,16 +1204,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1218,22 +1221,22 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N17" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>17</v>
@@ -1259,7 +1262,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>18</v>
@@ -1285,16 +1288,16 @@
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1311,13 +1314,13 @@
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>21</v>
@@ -1337,16 +1340,16 @@
         <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1354,10 +1357,10 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="6" t="s">
@@ -1369,7 +1372,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>18</v>
@@ -1395,13 +1398,13 @@
         <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E24" s="8">
         <v>2</v>
@@ -1412,7 +1415,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -1423,13 +1426,13 @@
         <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E25" s="8">
         <v>1</v>
@@ -1449,13 +1452,13 @@
         <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E26" s="8">
         <v>1</v>
@@ -1466,7 +1469,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -1477,7 +1480,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>17</v>
@@ -1501,10 +1504,10 @@
         <v>15</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>18</v>
@@ -1518,7 +1521,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -1529,10 +1532,10 @@
         <v>15</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>18</v>
@@ -1630,7 +1633,7 @@
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="6"/>
@@ -1646,7 +1649,7 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="6"/>
@@ -1662,7 +1665,7 @@
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="6"/>
@@ -1678,7 +1681,7 @@
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="6"/>
@@ -1694,7 +1697,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="6"/>
@@ -1710,7 +1713,7 @@
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="6"/>

</xml_diff>

<commit_message>
reattemp Best time to buy & sell and valid anagram
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -136,9 +136,6 @@
     <t>Affirm, Spotify</t>
   </si>
   <si>
-    <t>1*</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
     <t>Amex, Wayfair, Yandex</t>
   </si>
   <si>
+    <t>1*</t>
+  </si>
+  <si>
     <t>Not Sure</t>
   </si>
   <si>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t>Adobe, Alation, Amazon, Apple, Atlassian, Bloomberg, ByteDance, Capital One, Cisco, Docusign, Expedia, Goldman Sachs, JP Morgan, Netflix, Orcale, Paypal, ServiceNow, Uber, Visa, Walmart, Zoho, Zoom, eBay, tcs</t>
-  </si>
-  <si>
-    <t>4*</t>
   </si>
   <si>
     <t xml:space="preserve">Snapshot Array </t>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>Reverse Linked List (Recursively)</t>
+  </si>
+  <si>
+    <t>4*</t>
   </si>
   <si>
     <t xml:space="preserve">Has Cycle </t>
@@ -711,7 +711,7 @@
     <col min="14" max="14" style="10" width="16.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -755,7 +755,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -859,7 +859,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -887,7 +887,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -915,7 +915,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>39</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1080,7 +1080,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -1088,16 +1088,16 @@
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1125,7 +1125,7 @@
         <v>46</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1144,13 +1144,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="E15" s="8">
         <v>3</v>
@@ -1172,7 +1172,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>17</v>
@@ -1189,10 +1189,10 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L16" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="6" t="s">
@@ -1204,16 +1204,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1221,22 +1221,22 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="L17" s="6" t="s">
+      <c r="M17" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="N17" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>17</v>
@@ -1262,7 +1262,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>18</v>
@@ -1288,16 +1288,16 @@
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1314,16 +1314,16 @@
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -1349,7 +1349,7 @@
         <v>67</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1507,7 +1507,7 @@
         <v>76</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>18</v>
@@ -1535,7 +1535,7 @@
         <v>77</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
added largest parimeter triangle
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="80">
   <si>
     <t>Src</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>Increasing Triplet Subsequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Largest Perimeter Triangle </t>
+  </si>
+  <si>
+    <t>Tesla</t>
   </si>
 </sst>
 </file>
@@ -1554,10 +1560,18 @@
       <c r="N29" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="A30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>

</xml_diff>

<commit_message>
Added delete node in a linkedlist
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="84">
   <si>
     <t>Src</t>
   </si>
@@ -263,6 +263,12 @@
   </si>
   <si>
     <t>Diameter of Binary Tree</t>
+  </si>
+  <si>
+    <t>Delete Node in a Linked List</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -723,7 +729,7 @@
     <col min="14" max="14" style="10" width="16.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -767,7 +773,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -871,7 +877,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -899,7 +905,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -927,7 +933,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -1027,7 +1033,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -1642,17 +1648,29 @@
       <c r="N32" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="3"/>
+      <c r="A33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="8">
+        <v>1</v>
+      </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
+      <c r="K33" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>

</xml_diff>

<commit_message>
added: delete middle node of LinkedList
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="84">
   <si>
     <t>Src</t>
   </si>
@@ -268,7 +268,7 @@
     <t>Delete Node in a Linked List</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>Delete the Middle Node of a Linked List</t>
   </si>
 </sst>
 </file>
@@ -1263,7 +1263,7 @@
         <v>18</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1341,7 +1341,7 @@
         <v>54</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -1425,7 +1425,7 @@
         <v>72</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1479,7 +1479,7 @@
         <v>72</v>
       </c>
       <c r="E26" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1658,7 +1658,7 @@
         <v>48</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="E33" s="8">
         <v>1</v>
@@ -1676,8 +1676,12 @@
       <c r="N33" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="3"/>

</xml_diff>

<commit_message>
Added: Check if sentence is a panagram
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="85">
   <si>
     <t>Src</t>
   </si>
@@ -145,9 +145,6 @@
     <t>Amex, Wayfair, Yandex</t>
   </si>
   <si>
-    <t>1*</t>
-  </si>
-  <si>
     <t>Not Sure</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
     <t>Binary Tree In Order Traversal</t>
   </si>
   <si>
+    <t>1*</t>
+  </si>
+  <si>
     <t>Diameter of Binary Tree</t>
   </si>
   <si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>Delete the Middle Node of a Linked List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check if sentence is a pangram </t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1118,7 @@
         <v>42</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1126,7 +1129,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
@@ -1134,13 +1137,13 @@
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>31</v>
@@ -1154,7 +1157,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
@@ -1162,13 +1165,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="E15" s="8">
         <v>3</v>
@@ -1190,7 +1193,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>17</v>
@@ -1207,14 +1210,14 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
@@ -1222,16 +1225,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>55</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1239,22 +1242,22 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="L17" s="6" t="s">
+      <c r="M17" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="N17" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>17</v>
@@ -1280,7 +1283,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>18</v>
@@ -1306,16 +1309,16 @@
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1332,13 +1335,13 @@
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>28</v>
@@ -1358,16 +1361,16 @@
         <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1375,10 +1378,10 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="6" t="s">
@@ -1390,7 +1393,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>18</v>
@@ -1416,13 +1419,13 @@
         <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>31</v>
@@ -1433,7 +1436,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -1444,13 +1447,13 @@
         <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E25" s="8">
         <v>1</v>
@@ -1470,13 +1473,13 @@
         <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E26" s="8">
         <v>2</v>
@@ -1487,7 +1490,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -1498,7 +1501,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>17</v>
@@ -1522,10 +1525,10 @@
         <v>15</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>18</v>
@@ -1539,7 +1542,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -1550,10 +1553,10 @@
         <v>15</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>18</v>
@@ -1576,13 +1579,13 @@
         <v>15</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E30" s="8">
         <v>1</v>
@@ -1602,7 +1605,7 @@
         <v>15</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>17</v>
@@ -1611,7 +1614,7 @@
         <v>18</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -1655,7 +1658,7 @@
         <v>82</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>18</v>
@@ -1669,7 +1672,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -1696,10 +1699,18 @@
       <c r="N34" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
+      <c r="A35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>

</xml_diff>

<commit_message>
Added count and say to database
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="87">
   <si>
     <t>Src</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>Balanced Binary Tree</t>
+  </si>
+  <si>
+    <t>Count and say</t>
   </si>
 </sst>
 </file>
@@ -1756,8 +1759,12 @@
       <c r="N36" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="3"/>
@@ -1819,7 +1826,7 @@
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="6"/>
@@ -1835,7 +1842,7 @@
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="6"/>
@@ -1851,7 +1858,7 @@
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="6"/>
@@ -1867,7 +1874,7 @@
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="6"/>
@@ -1883,7 +1890,7 @@
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="6"/>
@@ -1899,7 +1906,7 @@
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="6"/>
@@ -1915,7 +1922,7 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="6"/>
@@ -1931,7 +1938,7 @@
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="6"/>
@@ -1947,7 +1954,7 @@
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="6"/>

</xml_diff>

<commit_message>
added questions to list
</commit_message>
<xml_diff>
--- a/Leetcode Tracker.xlsx
+++ b/Leetcode Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="100">
   <si>
     <t>Src</t>
   </si>
@@ -305,6 +305,18 @@
   </si>
   <si>
     <t>Airbnb(6), Lyft(9)</t>
+  </si>
+  <si>
+    <t>Subtree of another tree</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subtree-of-another-tree/discuss/265239/Python-Easy-to-Understand</t>
+  </si>
+  <si>
+    <t>Check if two string array are equivalent</t>
   </si>
 </sst>
 </file>
@@ -1930,13 +1942,27 @@
       <c r="N42" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
+      <c r="A43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="8">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="H43" s="3"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -1946,9 +1972,15 @@
       <c r="N43" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="6"/>
+      <c r="A44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="D44" s="6"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>

</xml_diff>